<commit_message>
Generating excel summary files for loads
</commit_message>
<xml_diff>
--- a/StagingTemplates/Errors.xlsx
+++ b/StagingTemplates/Errors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\CARE Somalia\Data\StagingTemplates\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\GitHub\Meerkat\StagingTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>QueueID</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>PackageErrorColumn</t>
+  </si>
+  <si>
+    <t>BusinessKey</t>
   </si>
 </sst>
 </file>
@@ -370,10 +373,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -384,7 +387,7 @@
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -401,6 +404,9 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>